<commit_message>
Updated debug vplan with pass/fail criteria and test type.
Signed-off-by: Oystein Knauserud <Oystein.Knauserud@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/debug-trace/CV32E40P_debug.xlsx
+++ b/verif/CV32E40P/VerificationPlan/debug-trace/CV32E40P_debug.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oyknause\Dropbox (Silicon Labs)\OpenHW Verif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\home\oyknause\openhw\core-v-docs\verif\CV32E40P\VerificationPlan\debug-trace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C066A40-F443-4304-86F2-7BC7778F2ABB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2514A7BE-F165-48D8-9E83-4271FCF238B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20840" yWindow="-9890" windowWidth="31330" windowHeight="14840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19350" yWindow="-10340" windowWidth="31630" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="141">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -1823,10 +1823,19 @@
     </r>
   </si>
   <si>
-    <t>CV32E40P XLEN=1 (32 bits).  DXLEN is defined as the widest supported XLEN. For now, this will be 1 (32 bits).</t>
-  </si>
-  <si>
     <t>Fence instructions</t>
+  </si>
+  <si>
+    <t>Requires virtual peripheral to generate irq</t>
+  </si>
+  <si>
+    <t>CV32E40P XLEN=1 (32 bits).  DXLEN is defined as the widest supported XLEN. For now, this will be 1 (32 bits). Check XLEN M- and D-mode</t>
+  </si>
+  <si>
+    <t>Requires a delay in the virtual peripheral to allow core to start execute WFI before debug_req is asserted</t>
+  </si>
+  <si>
+    <t>Requires tb to make virtual peripheral assert debug req before releasing reset</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1949,9 +1958,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1971,9 +1977,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1983,6 +1986,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2368,28 +2389,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AML68"/>
+  <dimension ref="A1:AML89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="33.36328125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="51.1796875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="45" style="14" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="31" style="14" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="54.54296875" style="14" customWidth="1"/>
-    <col min="11" max="1024" width="17" style="14" customWidth="1"/>
-    <col min="1025" max="1026" width="9.1796875" style="14" customWidth="1"/>
-    <col min="1027" max="16384" width="8.81640625" style="13"/>
+    <col min="1" max="1" width="23.453125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="33.36328125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="51.1796875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="45" style="13" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="31" style="13" customWidth="1"/>
+    <col min="9" max="9" width="22.81640625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="54.54296875" style="13" customWidth="1"/>
+    <col min="11" max="11" width="40.36328125" style="13" customWidth="1"/>
+    <col min="12" max="1024" width="17" style="13" customWidth="1"/>
+    <col min="1025" max="1026" width="9.1796875" style="13" customWidth="1"/>
+    <col min="1027" max="16384" width="8.81640625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -2425,1056 +2446,1630 @@
       </c>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:11" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E4" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" ht="250" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="G4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E6" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F6" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" s="6" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="D8" s="20"/>
+      <c r="E8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F8" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="G8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" s="6" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="G10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C12" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="G12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B14" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C14" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D14" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E14" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F14" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="G14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C16" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E16" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="G16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B18" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C18" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D18" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F18" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="G18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B22" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C22" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D22" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E22" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F22" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="G22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B24" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C24" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D24" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E24" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F24" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="G24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="D26" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B30" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C30" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D30" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E30" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="F30" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11" t="s">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B33" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C33" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D33" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E33" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F33" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="G33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B35" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C35" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D35" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E35" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
+      <c r="G35" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="20"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B37" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C37" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D37" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F37" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="6" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="G37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="6" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B39" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C39" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D39" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E39" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F39" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="6" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+      <c r="G39" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="6" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="20"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="6" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B41" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C41" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D41" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E41" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F41" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="G41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="6" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="20"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E43" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F43" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B44" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C44" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D44" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E44" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F44" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+      <c r="G44" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="20"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B46" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C46" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D46" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E46" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F46" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
+      <c r="G46" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="20"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B48" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C48" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D48" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E48" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F48" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="G48" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="20"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B50" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C50" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D50" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E50" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F50" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="6" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
+      <c r="G50" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="20"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" s="6" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A52" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11" t="s">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-    </row>
-    <row r="36" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-    </row>
-    <row r="37" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-    </row>
-    <row r="47" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-    </row>
-    <row r="49" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-    </row>
-    <row r="50" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-    </row>
-    <row r="52" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-    </row>
-    <row r="53" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-    </row>
-    <row r="54" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-    </row>
-    <row r="56" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-    </row>
-    <row r="57" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-    </row>
-    <row r="58" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-    </row>
-    <row r="59" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-    </row>
-    <row r="60" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-    </row>
-    <row r="61" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-    </row>
-    <row r="62" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-    </row>
-    <row r="63" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-    </row>
-    <row r="64" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-    </row>
-    <row r="65" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-    </row>
-    <row r="66" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-    </row>
-    <row r="67" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-    </row>
-    <row r="68" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="19" t="s">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+    </row>
+    <row r="65" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+    </row>
+    <row r="81" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+    </row>
+    <row r="84" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+    </row>
+    <row r="85" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+    </row>
+    <row r="86" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+    </row>
+    <row r="87" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+    </row>
+    <row r="88" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+    </row>
+    <row r="89" spans="2:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+      <c r="J89" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B68:J68"/>
+  <mergeCells count="127">
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B89:J89"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3486,19 +4081,19 @@
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G67</xm:sqref>
+          <xm:sqref>G2:G88</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C1B4F20-53D1-4A1B-832B-6E8BECAAA5F1}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H67</xm:sqref>
+          <xm:sqref>H2:H88</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79222D68-7559-4143-9FDD-D11E5D5A8DF0}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I67</xm:sqref>
+          <xm:sqref>I2:I88</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3611,47 +4206,47 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some extra info and TBDs in the debug vplan
Signed-off-by: Oystein Knauserud <Oystein.Knauserud@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/debug-trace/CV32E40P_debug.xlsx
+++ b/verif/CV32E40P/VerificationPlan/debug-trace/CV32E40P_debug.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\home\oyknause\openhw\core-v-docs\verif\CV32E40P\VerificationPlan\debug-trace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2514A7BE-F165-48D8-9E83-4271FCF238B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30872CF-D88A-4A71-B521-2F126F0B79FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19350" yWindow="-10340" windowWidth="31630" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -382,32 +382,6 @@
     <t>Exceptions</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">While in debug mode and executing from the program buffer, exceptions don’t update any registers but they </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> end execution of PB (go back to M-mode (?))</t>
-    </r>
-  </si>
-  <si>
     <t>Bring core into debug mode and start executing from program buffer. Make sure PB includes code that will hit an exception. Make sure core doesn’t update any registers, and jumps out of debug mode into M-mode</t>
   </si>
   <si>
@@ -624,12 +598,1146 @@
   </si>
   <si>
     <t>N/A for CV32E40P (requires A-extention)</t>
+  </si>
+  <si>
+    <t>While in debug mode and executing from the program buffer, no action is taken on any trigger match.</t>
+  </si>
+  <si>
+    <t>Bring core into debug and enable a trigger on the PC (pointing to the debug program buffer). Continue execution in debug, and observe that no action is taken when the trigger matches.</t>
+  </si>
+  <si>
+    <t>Program Buffer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Counters </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>may</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be stopped, depending on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">stopcount </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dscr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Timers </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>may</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be stopped, depending on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">stoptime </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All control transfer instructions </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>may act</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as illegal instructions if destination is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>within</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> program buffer. If one does, all must.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">By setting </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>step</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> before resuming execution, a debugger can cause the hart to execute a single instructin before re-entering debug mode.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bring the hart into debug mode. Set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>step</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bit in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and then resume execution. Observe that the hart runs a single instruction and the goes back to debug mode.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the instruction being fetched or executed in a single step causes a trigger, debug mode is entered immediately after the trigger fired. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cause</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is set to 2 instead of 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the instruction being fetched or executed in a single step casues an exception, debug mode is entered immediately </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">after </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the PC is changed to the exception handler and registers </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cause</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are updated.</t>
+    </r>
+  </si>
+  <si>
+    <t>If the intruction executed in the single step results in a PC that will cause an exception, the exception will not execute until the next time the hart resumes.</t>
+  </si>
+  <si>
+    <t>If the intruction executed in the single step results in a PC that will cause a trigger event, the trigger event will not take place until the instruction is executed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the single step instruction is WFI, it must be treated as a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instead of stalling and waiting for interrupt.</t>
+    </r>
+  </si>
+  <si>
+    <t>4.5 Reset</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When the hart comes out of reset, it must immediately enter debug mode without executing any instructions if the halt signal or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resethalterq</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is asserted.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.6 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Executing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> while NOT in debug mode will cause an illegal instruction exception.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Insert </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> into arbitrary code running in m-mode, observe that the illegal insctruction exception is thrown.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Executing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> while in debug mode will restore PC to the value in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dpc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and exit debug mode. (privilege level will be restored to the value in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bring hart into debug mode. Execute a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction and observe that the hart resumes executing from the correct address as given by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dpc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Debug mode can be entered by asserting the external signal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>debug_req_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">i
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cause</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The CV32E40P contains a trigger module with a single trigger register capable of triggering on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>instruction address match</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Write '1' to tdata1[2] to enable matching
+Write breakpoint addr to tdata2 register
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cause</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 2</t>
+    </r>
+  </si>
+  <si>
+    <t>Bring core into debug mode and start executing from program buffer. Generate interrupts (including NMI) and ensure they are masked.</t>
+  </si>
+  <si>
+    <t>Copyright 202[x] Silicon Labs Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>This document, all associated software, and derivatives thereof are licensed under the Solderpad License, Version 2.0 (the "License").</t>
+  </si>
+  <si>
+    <t>Use of this file means you agree to the terms and conditions of the License and are in full compliance with the License.</t>
+  </si>
+  <si>
+    <t>You may obtain a copy of the License at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      https://solderpad.org/licenses/SHL-2.0/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t>Unless required by applicable law or agreed to in writing, software and hardware implementations thereof distributed under the License is distributed on an "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>AS IS" BASIS, WITHOUT WARRANTIES OR CONDITIONS OF ANY KIND,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EITHER EXPRESSED OR IMPLIED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>See the License for the specific language governing permissions and limitations under the License.</t>
+  </si>
+  <si>
+    <t>RISC-V External Debug Support Version 0.13.2</t>
+  </si>
+  <si>
+    <t>RISC-V ISM vol 1 (unpriv. ISA), 20191213</t>
+  </si>
+  <si>
+    <t>Semihosting</t>
+  </si>
+  <si>
+    <t>To enable semihosting, a special instruction sequence is needed as there is only a single EBREAK instruction available.
+slli x0, x0, 0x1f # Entry NOP
+ebreak # Break to debugger
+srai x0, x0, 7 # NOP encoding the semihosting call number 7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bring hart into debug mode and start executing from the Program Buffer. Make sure the PB code includes an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ebreak</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction. When the ebreak is executed, the hart must halt and not update </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dpc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Perform a single step. Make sure the instruction executed in the step will cause an exception. PC must jump to the exception handler address and update </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cause</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and then immediately enter debug mode.</t>
+    </r>
+  </si>
+  <si>
+    <t>Make sure that an instruction in the instruction memory will generate a PC that causes an exception. Set up single stepping and make sure to step through this specific instruction. Hart must go back to debug mode after stepping, and the exception must not start executing until the next time the hart resumes (either single step or exit debug mode)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set up the trigger module to match on instruction address. Set up single stepping such that the match address will be executed in a step. The trigger module must fire during the step, and debug mode entered with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cause = 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to identify that the trigger was fired. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(#1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This can be verified in the same steps as marked with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(#1).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Perform a single step where the instruction to be executed is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WFI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction. The hart must not wait for interrupt, but treat the instruction as as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and re-enter debug after finishing the step.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assert the core reset AND the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>debug_req_i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> signal. The hart must not execute any instructions, but immediately enter debug mode.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fence instructions</t>
+  </si>
+  <si>
+    <t>Requires virtual peripheral to generate irq</t>
+  </si>
+  <si>
+    <t>CV32E40P XLEN=1 (32 bits).  DXLEN is defined as the widest supported XLEN. For now, this will be 1 (32 bits). Check XLEN M- and D-mode</t>
+  </si>
+  <si>
+    <t>Requires a delay in the virtual peripheral to allow core to start execute WFI before debug_req is asserted</t>
+  </si>
+  <si>
+    <t>Requires tb to make virtual peripheral assert debug req before releasing reset</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TBD - need to understand the fence instruction. Is "completing program buffer execution" the same as executing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Insert </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WFI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction into arbitrary code. While the hart is waiting for an interrupt, request debug mode. The hart must stop waiting for interrupt and enter debug mode. What if WFI is at the trigger address?</t>
+    </r>
   </si>
   <si>
     <r>
       <t xml:space="preserve">Verify that core enters debug mode when the trigger matches on instruction address. NB! According to spec, the tdataN registers can only be written from debug mode, as m-mode writes are ignored.
 Enter debug mode by any of the above methods.
-Write breakpoint addr to tdata2 and enable breakpoint in tdata1[2]
+Write (randomized) breakpoint addr to tdata2 and enable breakpoint in tdata1[2]
 Exit debug mode (dret instruction)
 Verify that core enters debug mode on breakpoint addr
 Current PC is saved to DPC
@@ -659,640 +1767,55 @@
     </r>
   </si>
   <si>
-    <t>While in debug mode and executing from the program buffer, no action is taken on any trigger match.</t>
-  </si>
-  <si>
-    <t>Bring core into debug and enable a trigger on the PC (pointing to the debug program buffer). Continue execution in debug, and observe that no action is taken when the trigger matches.</t>
-  </si>
-  <si>
-    <t>Program Buffer</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Counters </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>may</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be stopped, depending on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">stopcount </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dscr</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Timers </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>may</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be stopped, depending on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">stoptime </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">All control transfer instructions </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>may act</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as illegal instructions if destination is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>within</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> program buffer. If one does, all must.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">By setting </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>step</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr[2]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> before resuming execution, a debugger can cause the hart to execute a single instructin before re-entering debug mode.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bring the hart into debug mode. Set the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>step</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bit in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr[2]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and then resume execution. Observe that the hart runs a single instruction and the goes back to debug mode.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If the instruction being fetched or executed in a single step causes a trigger, debug mode is entered immediately after the trigger fired. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cause</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is set to 2 instead of 4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If the instruction being fetched or executed in a single step casues an exception, debug mode is entered immediately </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">after </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">the PC is changed to the exception handler and registers </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>tval</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cause</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> are updated.</t>
-    </r>
-  </si>
-  <si>
-    <t>If the intruction executed in the single step results in a PC that will cause an exception, the exception will not execute until the next time the hart resumes.</t>
-  </si>
-  <si>
-    <t>If the intruction executed in the single step results in a PC that will cause a trigger event, the trigger event will not take place until the instruction is executed.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If the single step instruction is WFI, it must be treated as a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nop</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instead of stalling and waiting for interrupt.</t>
-    </r>
-  </si>
-  <si>
-    <t>4.5 Reset</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When the hart comes out of reset, it must immediately enter debug mode without executing any instructions if the halt signal or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>resethalterq</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is asserted.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4.6 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Executing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> while NOT in debug mode will cause an illegal instruction exception.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Insert </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> into arbitrary code running in m-mode, observe that the illegal insctruction exception is thrown.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Executing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> while in debug mode will restore PC to the value in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dpc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and exit debug mode. (privilege level will be restored to the value in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bring hart into debug mode. Execute a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction and observe that the hart resumes executing from the correct address as given by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dpc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
+    <r>
+      <t xml:space="preserve">Bring core into debug mode, generate all exception types and observe that the PC jumps to the address given by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dm_exception_addr_i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Observe no change in status registers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">While in debug mode and executing from the program buffer, exceptions don’t update any registers but they </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> end execution of PB (TBD: goes back to M-mode or restarts in debug(?))</t>
     </r>
   </si>
   <si>
@@ -1340,33 +1863,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Debug mode can be entered by asserting the external signal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>debug_req_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">i
+      <t xml:space="preserve"> = 1
 </t>
     </r>
     <r>
@@ -1378,45 +1875,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>cause</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The CV32E40P contains a trigger module with a single trigger register capable of triggering on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>instruction address match</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-Write '1' to tdata1[2] to enable matching
-Write breakpoint addr to tdata2 register
+      <t>TBD:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> What happens when dcsr.ebreakm = 0 ?
 </t>
     </r>
     <r>
@@ -1428,414 +1897,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>cause</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bring core into debug mode, generate an exception and observe that the PC jumps to the address given by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dm_exception_addr_i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Observe no change in status registers</t>
-    </r>
-  </si>
-  <si>
-    <t>Bring core into debug mode and start executing from program buffer. Generate interrupts (including NMI) and ensure they are masked.</t>
-  </si>
-  <si>
-    <t>Copyright 202[x] Silicon Labs Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>This document, all associated software, and derivatives thereof are licensed under the Solderpad License, Version 2.0 (the "License").</t>
-  </si>
-  <si>
-    <t>Use of this file means you agree to the terms and conditions of the License and are in full compliance with the License.</t>
-  </si>
-  <si>
-    <t>You may obtain a copy of the License at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      https://solderpad.org/licenses/SHL-2.0/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <r>
-      <t>Unless required by applicable law or agreed to in writing, software and hardware implementations thereof distributed under the License is distributed on an "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>AS IS" BASIS, WITHOUT WARRANTIES OR CONDITIONS OF ANY KIND,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>EITHER EXPRESSED OR IMPLIED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>See the License for the specific language governing permissions and limitations under the License.</t>
-  </si>
-  <si>
-    <t>RISC-V External Debug Support Version 0.13.2</t>
-  </si>
-  <si>
-    <t>RISC-V ISM vol 1 (unpriv. ISA), 20191213</t>
-  </si>
-  <si>
-    <t>Semihosting</t>
-  </si>
-  <si>
-    <t>To enable semihosting, a special instruction sequence is needed as there is only a single EBREAK instruction available.
-slli x0, x0, 0x1f # Entry NOP
-ebreak # Break to debugger
-srai x0, x0, 7 # NOP encoding the semihosting call number 7</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bring hart into debug mode and start executing from the Program Buffer. Make sure the PB code includes an </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ebreak</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction. When the ebreak is executed, the hart must halt and not update </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dpc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Insert </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WFI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction into arbitrary code. While the hart is waiting for an interrupt, request debug mode. The hart must stop waiting for interrupt and enter debug mode.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Perform a single step. Make sure the instruction executed in the step will cause an exception. PC must jump to the exception handler address and update </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>tval</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cause</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and then immediately enter debug mode.</t>
-    </r>
-  </si>
-  <si>
-    <t>Make sure that an instruction in the instruction memory will generate a PC that causes an exception. Set up single stepping and make sure to step through this specific instruction. Hart must go back to debug mode after stepping, and the exception must not start executing until the next time the hart resumes (either single step or exit debug mode)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set up the trigger module to match on instruction address. Set up single stepping such that the match address will be executed in a step. The trigger module must fire during the step, and debug mode entered with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cause = 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to identify that the trigger was fired. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(#1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This can be verified in the same steps as marked with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(#1).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Perform a single step where the instruction to be executed is a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WFI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction. The hart must not wait for interrupt, but treat the instruction as as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and re-enter debug after finishing the step.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Assert the core reset AND the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>debug_req_i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signal. The hart must not execute any instructions, but immediately enter debug mode.</t>
-    </r>
-  </si>
-  <si>
-    <t>Fence instructions</t>
-  </si>
-  <si>
-    <t>Requires virtual peripheral to generate irq</t>
-  </si>
-  <si>
-    <t>CV32E40P XLEN=1 (32 bits).  DXLEN is defined as the widest supported XLEN. For now, this will be 1 (32 bits). Check XLEN M- and D-mode</t>
-  </si>
-  <si>
-    <t>Requires a delay in the virtual peripheral to allow core to start execute WFI before debug_req is asserted</t>
-  </si>
-  <si>
-    <t>Requires tb to make virtual peripheral assert debug req before releasing reset</t>
+      <t xml:space="preserve">TBD: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What about EBREAKM inside exceptions?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2389,10 +2462,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AML89"/>
+  <dimension ref="A1:AML90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2460,7 +2533,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>36</v>
@@ -2472,7 +2545,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
@@ -2506,7 +2579,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>37</v>
@@ -2518,7 +2591,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -2554,10 +2627,10 @@
         <v>33</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>10</v>
@@ -2566,11 +2639,11 @@
         <v>16</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -2603,7 +2676,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>10</v>
@@ -2612,7 +2685,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8" s="7"/>
     </row>
@@ -2658,7 +2731,7 @@
         <v>17</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10" s="7"/>
     </row>
@@ -2704,7 +2777,7 @@
         <v>16</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12" s="7"/>
     </row>
@@ -2728,22 +2801,22 @@
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>10</v>
@@ -2752,10 +2825,10 @@
         <v>16</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -2778,22 +2851,22 @@
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>50</v>
       </c>
       <c r="E16" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>10</v>
@@ -2802,7 +2875,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K16" s="7"/>
     </row>
@@ -2826,22 +2899,22 @@
     </row>
     <row r="18" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>10</v>
@@ -2850,7 +2923,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K18" s="7"/>
     </row>
@@ -2874,22 +2947,22 @@
     </row>
     <row r="20" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -2900,22 +2973,22 @@
     </row>
     <row r="21" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="F21" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -2926,22 +2999,22 @@
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>10</v>
@@ -2950,7 +3023,7 @@
         <v>16</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22" s="7"/>
     </row>
@@ -2974,22 +3047,22 @@
     </row>
     <row r="24" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>128</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>10</v>
@@ -2998,7 +3071,7 @@
         <v>16</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K24" s="7"/>
     </row>
@@ -3020,23 +3093,25 @@
       </c>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="6" t="s">
@@ -3046,22 +3121,22 @@
     </row>
     <row r="27" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -3072,22 +3147,22 @@
     </row>
     <row r="28" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -3098,22 +3173,22 @@
     </row>
     <row r="29" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -3124,22 +3199,22 @@
     </row>
     <row r="30" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>10</v>
@@ -3148,7 +3223,7 @@
         <v>16</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K30" s="7"/>
     </row>
@@ -3165,16 +3240,16 @@
     </row>
     <row r="32" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -3184,22 +3259,22 @@
     </row>
     <row r="33" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B33" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>83</v>
-      </c>
       <c r="F33" s="20" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>10</v>
@@ -3208,10 +3283,10 @@
         <v>16</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -3233,22 +3308,22 @@
     </row>
     <row r="35" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B35" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>85</v>
-      </c>
       <c r="E35" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>10</v>
@@ -3257,7 +3332,7 @@
         <v>16</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -3279,22 +3354,22 @@
     </row>
     <row r="37" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B37" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>85</v>
-      </c>
       <c r="E37" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>10</v>
@@ -3303,7 +3378,7 @@
         <v>16</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -3325,22 +3400,22 @@
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B39" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>85</v>
-      </c>
       <c r="E39" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>10</v>
@@ -3349,7 +3424,7 @@
         <v>16</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="6" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3371,22 +3446,22 @@
     </row>
     <row r="41" spans="1:11" s="6" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B41" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>85</v>
-      </c>
       <c r="E41" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>10</v>
@@ -3395,7 +3470,7 @@
         <v>16</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
@@ -3415,236 +3490,253 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" s="6" t="s">
+    <row r="43" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="E43" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="I43" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" s="21" t="s">
+    <row r="44" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="20"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="G44" s="10" t="s">
+      <c r="E45" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="10" t="s">
+      <c r="I45" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="H46" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K46" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="20"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
+    </row>
+    <row r="47" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>130</v>
+      </c>
       <c r="G47" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="20"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="H48" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="20"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="G49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="20"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H50" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E50" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="20"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+    <row r="51" spans="1:9" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>107</v>
+      </c>
       <c r="G51" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="20"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H51" s="10"/>
-    </row>
-    <row r="52" spans="1:9" s="6" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A52" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B52" s="9" t="s">
+      <c r="H52" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A53" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-    </row>
-    <row r="53" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="10"/>
+      <c r="C53" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="E53" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
     </row>
@@ -3928,46 +4020,60 @@
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
     </row>
-    <row r="89" spans="2:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="17" t="s">
+    <row r="89" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+    </row>
+    <row r="90" spans="2:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
+      <c r="J90" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="127">
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
+  <mergeCells count="133">
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
     <mergeCell ref="F41:F42"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:C42"/>
@@ -4054,7 +4160,7 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B89:J89"/>
+    <mergeCell ref="B90:J90"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -4076,24 +4182,24 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDDA95CE-2B91-4BF6-A07B-87518765EC90}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G88</xm:sqref>
+          <xm:sqref>G2:G89</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C1B4F20-53D1-4A1B-832B-6E8BECAAA5F1}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H88</xm:sqref>
+          <xm:sqref>H2:H89</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79222D68-7559-4143-9FDD-D11E5D5A8DF0}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I88</xm:sqref>
+          <xm:sqref>I2:I89</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4207,47 +4313,47 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated debug vplan after meeting/discussion 2nd of July.
Signed-off-by: Oystein Knauserud <Oystein.Knauserud@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/debug-trace/CV32E40P_debug.xlsx
+++ b/verif/CV32E40P/VerificationPlan/debug-trace/CV32E40P_debug.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\home\oyknause\openhw\core-v-docs\verif\CV32E40P\VerificationPlan\debug-trace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30872CF-D88A-4A71-B521-2F126F0B79FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C0F315-3913-49CF-AC37-F7B01EF7868A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20110" yWindow="-10070" windowWidth="33560" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="146">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -445,9 +442,6 @@
     <t>Effective XLEN</t>
   </si>
   <si>
-    <t>N/A for CV32E40P</t>
-  </si>
-  <si>
     <t>In debug, the WFI instruction acts as a NOP instruction</t>
   </si>
   <si>
@@ -588,18 +582,12 @@
     <t>4.3 Wait for interrupt</t>
   </si>
   <si>
-    <t>If a halt is requsted while waiting for interrupt, WFI instruction must complete and hart enters debug mode.</t>
-  </si>
-  <si>
     <t>4.4 Single step</t>
   </si>
   <si>
     <t>Single stepping</t>
   </si>
   <si>
-    <t>N/A for CV32E40P (requires A-extention)</t>
-  </si>
-  <si>
     <t>While in debug mode and executing from the program buffer, no action is taken on any trigger match.</t>
   </si>
   <si>
@@ -825,53 +813,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Bring the hart into debug mode. Set the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>step</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bit in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr[2]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and then resume execution. Observe that the hart runs a single instruction and the goes back to debug mode.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">If the instruction being fetched or executed in a single step causes a trigger, debug mode is entered immediately after the trigger fired. </t>
     </r>
     <r>
@@ -1097,7 +1038,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Insert </t>
+      <t xml:space="preserve">Executing </t>
     </r>
     <r>
       <rPr>
@@ -1118,32 +1059,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> into arbitrary code running in m-mode, observe that the illegal insctruction exception is thrown.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Executing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> while in debug mode will restore PC to the value in </t>
     </r>
     <r>
@@ -1187,53 +1102,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bring hart into debug mode. Execute a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction and observe that the hart resumes executing from the correct address as given by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dpc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
     </r>
   </si>
   <si>
@@ -1576,22 +1444,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">This can be verified in the same steps as marked with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(#1).</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Perform a single step where the instruction to be executed is a </t>
     </r>
     <r>
@@ -1670,20 +1522,191 @@
     <t>Requires virtual peripheral to generate irq</t>
   </si>
   <si>
-    <t>CV32E40P XLEN=1 (32 bits).  DXLEN is defined as the widest supported XLEN. For now, this will be 1 (32 bits). Check XLEN M- and D-mode</t>
-  </si>
-  <si>
     <t>Requires a delay in the virtual peripheral to allow core to start execute WFI before debug_req is asserted</t>
   </si>
   <si>
     <t>Requires tb to make virtual peripheral assert debug req before releasing reset</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TBD - need to understand the fence instruction. Is "completing program buffer execution" the same as executing </t>
+    <r>
+      <t xml:space="preserve">Insert </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WFI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction into arbitrary code. While the hart is waiting for an interrupt, request debug mode. The hart must stop waiting for interrupt and enter debug mode. What if WFI is at the trigger address?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">While in debug mode and executing from the program buffer, exceptions don’t update any registers but they </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> end execution of PB (TBD: goes back to M-mode or restarts in debug(?))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Debug mode can be entered by executing the EBREAK or C.EBREAK instruction when </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr.ebreakm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cause</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TBD:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> What happens when dcsr.ebreakm = 0 ?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TBD: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What about EBREAKM inside exceptions?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bring core into debug mode, generate all exception types and observe that the PC jumps to the address given by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dm_exception_addr_i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Observe no change in status registers
+According to specification, the cf32e40p supports the following types of exceptions:
+Illegal instruction (2)
+Breakpoint (3)
+Environment call from M-mode (ECALL) (11)</t>
+    </r>
+  </si>
+  <si>
+    <t>If all points above passes, there should be nothing to verify here. Semihosting will be handled from SW.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Insert </t>
     </r>
     <r>
       <rPr>
@@ -1704,33 +1727,141 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> into arbitrary code running in m-mode, observe that the illegal insctruction exception is thrown.
+Can be tested in the same test as for debug entry</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bring hart into debug mode. Execute a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction and observe that the hart resumes executing from the correct address as given by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dpc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 
+Can be tested in the same test as for debug entry.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">debug_req_i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is asserted while waiting for interrupt, WFI instruction must complete and hart enters debug mode.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TBD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - need to understand the fence instruction in cv32e40p. Is "completing program buffer execution" the same as executing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>?</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Insert </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WFI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instruction into arbitrary code. While the hart is waiting for an interrupt, request debug mode. The hart must stop waiting for interrupt and enter debug mode. What if WFI is at the trigger address?</t>
+      <t xml:space="preserve">N/A for CV32E40P : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>need Arjan/Davide to sign-off on this.</t>
     </r>
   </si>
   <si>
@@ -1751,6 +1882,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>dm_haltaddr_i</t>
     </r>
@@ -1760,7 +1892,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> input
 Core starts executing debug code</t>
@@ -1768,146 +1900,173 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Bring core into debug mode, generate all exception types and observe that the PC jumps to the address given by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dm_exception_addr_i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Observe no change in status registers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">While in debug mode and executing from the program buffer, exceptions don’t update any registers but they </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> end execution of PB (TBD: goes back to M-mode or restarts in debug(?))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Debug mode can be entered by executing the EBREAK or C.EBREAK instruction when </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dcsr.ebreakm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 1
+      <t xml:space="preserve">N/A for CV32E40P </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> need Arjan/Davide to sign-off on this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N/A for CV32E40P :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> need Arjan/Davide to sign-off on this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N/A for CV32E40P </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: need Arjan/Davide to sign-off on this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CV32E40P XLEN=1 (32 bits).  DXLEN is defined as the widest supported XLEN. For now, this will be 1 (32 bits). Check XLEN M- and D-mode
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cause</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 1
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mike: what exactly would a testcase actually do to check this?
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TBD:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> What happens when dcsr.ebreakm = 0 ?
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ØK: As discussed in the meeting 02.July, this is probably a SW/DM problem. Leaving it here for reference.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This can be verified in the same steps as marked with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(#1).
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">TBD: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What about EBREAKM inside exceptions?</t>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mike: this may be difficult to accurately predict in the ISS.  This is good input for the Imperas team.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N/A for CV32E40P (requires A-extention)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : need Arjan/Davide to sign-off on this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bring the hart into debug mode. Set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>step</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bit in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dcsr[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and then resume execution. Observe that the hart runs a single instruction and the goes back to debug mode.</t>
     </r>
   </si>
 </sst>
@@ -1915,7 +2074,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1989,8 +2148,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2003,6 +2191,12 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2013,11 +2207,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2057,6 +2252,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2066,21 +2277,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{1E1B0CF8-8C4F-41A9-9558-CBA9FC1B75F5}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2465,7 +2668,7 @@
   <dimension ref="A1:AML90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2520,22 +2723,22 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -2549,12 +2752,12 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="8" t="s">
         <v>24</v>
       </c>
@@ -2579,9 +2782,9 @@
         <v>31</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>37</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -2601,7 +2804,7 @@
       <c r="C5" s="21"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="18"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="10" t="s">
         <v>24</v>
       </c>
@@ -2627,10 +2830,10 @@
         <v>33</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>139</v>
+        <v>103</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>10</v>
@@ -2643,13 +2846,13 @@
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="175.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="22"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="10" t="s">
         <v>24</v>
       </c>
@@ -2676,7 +2879,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>10</v>
@@ -2689,7 +2892,7 @@
       </c>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="6" customFormat="1" ht="88.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="20"/>
@@ -2801,13 +3004,13 @@
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>53</v>
@@ -2816,7 +3019,7 @@
         <v>48</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>10</v>
@@ -2828,7 +3031,7 @@
         <v>20</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -2851,19 +3054,19 @@
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>50</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>51</v>
@@ -2899,22 +3102,22 @@
     </row>
     <row r="18" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>55</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>10</v>
@@ -2945,76 +3148,70 @@
       </c>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>10</v>
@@ -3047,22 +3244,22 @@
     </row>
     <row r="24" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>59</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>68</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>10</v>
@@ -3094,175 +3291,156 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="A26" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="6" t="s">
+      <c r="C26" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="18" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>69</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>69</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>70</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>64</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>71</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" s="6" customFormat="1" ht="94.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20"/>
       <c r="B31" s="21"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="33" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>54</v>
@@ -3271,10 +3449,10 @@
         <v>67</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>10</v>
@@ -3286,7 +3464,7 @@
         <v>20</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -3308,22 +3486,22 @@
     </row>
     <row r="35" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>145</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>10</v>
@@ -3335,13 +3513,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" s="6" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="20"/>
       <c r="B36" s="21"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="10" t="s">
         <v>24</v>
       </c>
@@ -3354,22 +3532,22 @@
     </row>
     <row r="37" spans="1:11" s="6" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>10</v>
@@ -3400,22 +3578,22 @@
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>10</v>
@@ -3446,22 +3624,22 @@
     </row>
     <row r="41" spans="1:11" s="6" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>10</v>
@@ -3492,22 +3670,22 @@
     </row>
     <row r="43" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>128</v>
+        <v>93</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>143</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>10</v>
@@ -3516,41 +3694,44 @@
         <v>16</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="F44" s="26"/>
       <c r="G44" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="I44" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="45" spans="1:11" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>10</v>
@@ -3581,22 +3762,22 @@
     </row>
     <row r="47" spans="1:11" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>10</v>
@@ -3608,7 +3789,7 @@
         <v>20</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -3630,22 +3811,22 @@
     </row>
     <row r="49" spans="1:9" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D49" s="23" t="s">
-        <v>103</v>
+      <c r="D49" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>10</v>
@@ -3661,7 +3842,7 @@
       <c r="A50" s="20"/>
       <c r="B50" s="21"/>
       <c r="C50" s="20"/>
-      <c r="D50" s="23"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
       <c r="G50" s="10" t="s">
@@ -3676,22 +3857,22 @@
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="23" t="s">
-        <v>103</v>
+      <c r="D51" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>10</v>
@@ -3707,7 +3888,7 @@
       <c r="A52" s="20"/>
       <c r="B52" s="21"/>
       <c r="C52" s="20"/>
-      <c r="D52" s="23"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
       <c r="G52" s="10" t="s">
@@ -3722,20 +3903,20 @@
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>136</v>
+        <v>117</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
@@ -4029,27 +4210,136 @@
       <c r="H89" s="10"/>
     </row>
     <row r="90" spans="2:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
+      <c r="J90" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="133">
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:C52"/>
@@ -4067,122 +4357,13 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDDA95CE-2B91-4BF6-A07B-87518765EC90}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$8</xm:f>
@@ -4313,47 +4494,47 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>